<commit_message>
Added status LED to "Beam Me Up" design
</commit_message>
<xml_diff>
--- a/Hardware/03 Beam Me Up/Parts List.xlsx
+++ b/Hardware/03 Beam Me Up/Parts List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>From</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>IC Socket</t>
+  </si>
+  <si>
+    <t>3mm LED</t>
+  </si>
+  <si>
+    <t>LED3R</t>
+  </si>
+  <si>
+    <t>100R Resistor</t>
+  </si>
+  <si>
+    <t>R100R14W</t>
   </si>
 </sst>
 </file>
@@ -182,8 +194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E12" totalsRowCount="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" totalsRowCount="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:E13"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Cat."/>
@@ -482,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -603,100 +615,135 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1">
+        <f>0.11/10</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="1">
         <f>0.07*4</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C10" s="1">
         <f>11.82+0.99*11.82/10.57</f>
         <v>12.927076631977295</v>
       </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>1.62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <f>6.32/2</f>
         <v>3.16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <f>3.2/5</f>
         <v>0.64</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C14" s="1">
         <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>21.422076631977298</v>
+        <v>21.513076631977299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added back-EMF protection to "Beam Me Up"
Also added the diodes for the back-EMF protection to the master parts
list.
</commit_message>
<xml_diff>
--- a/Hardware/03 Beam Me Up/Parts List.xlsx
+++ b/Hardware/03 Beam Me Up/Parts List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>From</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>R100R14W</t>
+  </si>
+  <si>
+    <t>1N4001</t>
+  </si>
+  <si>
+    <t>Diodes (x4)</t>
   </si>
 </sst>
 </file>
@@ -194,8 +200,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" totalsRowCount="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E15" totalsRowCount="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:E14"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Cat."/>
@@ -494,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -668,82 +674,100 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1">
+        <f>0.21/10*4</f>
+        <v>8.3999999999999991E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <f>11.82+0.99*11.82/10.57</f>
         <v>12.927076631977295</v>
       </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <f>6.32/2</f>
         <v>3.16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <f>3.2/5</f>
         <v>0.64</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>21.513076631977299</v>
+        <v>21.597076631977298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to parts lists
Received pager motors, added the PMV31XN MOSFETs which are on order.
</commit_message>
<xml_diff>
--- a/Hardware/03 Beam Me Up/Parts List.xlsx
+++ b/Hardware/03 Beam Me Up/Parts List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>From</t>
   </si>
@@ -91,18 +91,6 @@
     <t>Ok</t>
   </si>
   <si>
-    <t>Transistors (x4)</t>
-  </si>
-  <si>
-    <t>BC337</t>
-  </si>
-  <si>
-    <t>Use Damo's motors to test</t>
-  </si>
-  <si>
-    <t>Use HJ-998 props to test</t>
-  </si>
-  <si>
     <t>ICS28N</t>
   </si>
   <si>
@@ -127,7 +115,16 @@
     <t>Diodes (x4)</t>
   </si>
   <si>
-    <t>Use Damo's to test</t>
+    <t>MOSFETs (x4)</t>
+  </si>
+  <si>
+    <t>PMV31XN</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>RS Online</t>
   </si>
 </sst>
 </file>
@@ -505,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -555,10 +554,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1">
         <v>0.17</v>
@@ -624,10 +623,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
         <v>0.08</v>
@@ -641,10 +640,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <f>0.11/10</f>
@@ -659,38 +658,38 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
-        <f>0.07*4</f>
-        <v>0.28000000000000003</v>
+        <f>0.21/10*4</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1">
+        <f>0.286*4</f>
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="1">
-        <f>0.21/10*4</f>
-        <v>8.3999999999999991E-2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -770,7 +769,7 @@
       </c>
       <c r="C15" s="1">
         <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>21.597076631977298</v>
+        <v>22.461076631977296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>